<commit_message>
refactoring code/added search for client with regex/list client's invoices/added list of clients and invoices
</commit_message>
<xml_diff>
--- a/files/work_order.xlsx
+++ b/files/work_order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\OneDrive\Documentos\My projects\Musical Instruments Repair Shop System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\OneDrive\Documentos\My projects\Musical Instruments Repair Shop System\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F14C44-4E47-4B62-9807-863A5BA50119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6278F1F6-711C-4ADA-A62A-35130219F041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Work order</t>
   </si>
@@ -60,15 +60,6 @@
   </si>
   <si>
     <t>Anderson Ibanez RG</t>
-  </si>
-  <si>
-    <t>Date promised</t>
-  </si>
-  <si>
-    <t>Order Number</t>
-  </si>
-  <si>
-    <t>Date delivered</t>
   </si>
   <si>
     <t>567-09209</t>
@@ -109,6 +100,9 @@
   </si>
   <si>
     <t>012 Fantasy Street, Hogwarts, World - T1P0Z9 - (567) 891 2345 - goldenstr@luthier.com</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -121,7 +115,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -243,12 +237,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <i/>
       <sz val="9"/>
       <name val="Century Gothic"/>
@@ -261,6 +249,20 @@
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="7">
@@ -505,7 +507,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -601,10 +603,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -647,19 +649,24 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,8 +1195,8 @@
   </sheetPr>
   <dimension ref="B2:R40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1228,19 +1235,19 @@
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+    <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="4"/>
       <c r="F5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="22">
         <f ca="1">TODAY()</f>
-        <v>45137</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1279,34 +1286,30 @@
     </row>
     <row r="9" spans="2:7" s="6" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="45"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="21" t="s">
-        <v>8</v>
-      </c>
+      <c r="F10" s="21"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="46"/>
+      <c r="B11" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="57"/>
       <c r="D11" s="45"/>
       <c r="E11" s="46"/>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="46"/>
+      <c r="B12" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="57"/>
       <c r="D12" s="45"/>
       <c r="E12" s="46"/>
       <c r="F12" s="3"/>
@@ -1345,27 +1348,27 @@
     </row>
     <row r="17" spans="2:18" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27"/>
       <c r="C18" s="31"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="23"/>
       <c r="G18" s="24" t="str">
         <f t="shared" ref="G18:G31" si="0">IF(SUM(C18)&gt;0,SUM((C18*F18)),"")</f>
@@ -1535,7 +1538,7 @@
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
       <c r="F32" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G32" s="16" t="str">
         <f>IF(SUM(G18:G31)&gt;0,SUM(G18:G31),"")</f>
@@ -1544,13 +1547,13 @@
     </row>
     <row r="33" spans="2:7" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G33" s="17">
         <v>5</v>
@@ -1558,13 +1561,13 @@
     </row>
     <row r="34" spans="2:7" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
       <c r="F34" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G34" s="19" t="str">
         <f>IF(SUM(G32)&gt;0,SUM((G32*G33/100)+G32),"")</f>
@@ -1580,8 +1583,8 @@
       <c r="G35" s="9"/>
     </row>
     <row r="36" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="54" t="s">
-        <v>22</v>
+      <c r="B36" s="53" t="s">
+        <v>19</v>
       </c>
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
@@ -1591,7 +1594,7 @@
     </row>
     <row r="37" spans="2:7" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="49" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C37" s="50"/>
       <c r="D37" s="50"/>
@@ -1658,7 +1661,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup scale="85" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>